<commit_message>
Add manual clusters analysis tabular results. Add MSA based clusters analysis results that includes new brute force clustering algorithm
</commit_message>
<xml_diff>
--- a/data/tabular_data/swissprot clustering all algorithms manual analysis thpi 70.xlsx
+++ b/data/tabular_data/swissprot clustering all algorithms manual analysis thpi 70.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="130" documentId="09D1842FB96B8A63D6D4580CEC8B43A785CCD1F1" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{21E0D4F7-0CE8-4E90-B953-31F6B811829A}"/>
+  <xr:revisionPtr revIDLastSave="138" documentId="09D1842FB96B8A63D6D4580CEC8B43A785CCD1F1" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{B64D50E7-A438-4C87-AAA3-0ADD33DCE43D}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -377,7 +377,7 @@
   <dimension ref="A1:J51"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:J51"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -392,8 +392,9 @@
     <col min="8" max="8" width="18.5703125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="31.5703125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.28515625" customWidth="1"/>
-    <col min="13" max="13" width="38" customWidth="1"/>
+    <col min="11" max="11" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="35.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="20.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
@@ -433,31 +434,31 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C2">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="D2">
-        <v>85.990499999999997</v>
+        <v>85.042500000000004</v>
       </c>
       <c r="E2">
+        <v>88</v>
+      </c>
+      <c r="F2">
+        <v>66</v>
+      </c>
+      <c r="G2">
+        <v>83.649900000000002</v>
+      </c>
+      <c r="H2">
         <v>82</v>
       </c>
-      <c r="F2">
-        <v>74</v>
-      </c>
-      <c r="G2">
-        <v>86.629900000000006</v>
-      </c>
-      <c r="H2">
-        <v>85</v>
-      </c>
       <c r="I2">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="J2">
-        <v>85.990499999999997</v>
+        <v>85.042500000000004</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -465,31 +466,31 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>28</v>
+        <v>71</v>
       </c>
       <c r="C3">
-        <v>62</v>
+        <v>83</v>
       </c>
       <c r="D3">
-        <v>78.121700000000004</v>
+        <v>93.150499999999994</v>
       </c>
       <c r="E3">
-        <v>9</v>
+        <v>88</v>
       </c>
       <c r="F3">
+        <v>25</v>
+      </c>
+      <c r="G3">
+        <v>75.052999999999997</v>
+      </c>
+      <c r="H3">
         <v>71</v>
       </c>
-      <c r="G3">
-        <v>81.361099999999993</v>
-      </c>
-      <c r="H3">
-        <v>16</v>
-      </c>
       <c r="I3">
-        <v>12</v>
+        <v>83</v>
       </c>
       <c r="J3">
-        <v>85.75</v>
+        <v>93.150499999999994</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
@@ -497,31 +498,31 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>22</v>
+        <v>70</v>
       </c>
       <c r="C4">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="D4">
-        <v>82.359300000000005</v>
+        <v>89.166899999999998</v>
       </c>
       <c r="E4">
-        <v>19</v>
+        <v>86</v>
       </c>
       <c r="F4">
         <v>72</v>
       </c>
       <c r="G4">
-        <v>82.146199999999993</v>
+        <v>85.775099999999995</v>
       </c>
       <c r="H4">
-        <v>16</v>
+        <v>86</v>
       </c>
       <c r="I4">
         <v>72</v>
       </c>
       <c r="J4">
-        <v>81.55</v>
+        <v>85.775099999999995</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
@@ -529,31 +530,31 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>16</v>
+        <v>58</v>
       </c>
       <c r="C5">
-        <v>79</v>
+        <v>62</v>
       </c>
       <c r="D5">
-        <v>87.025000000000006</v>
+        <v>77.826400000000007</v>
       </c>
       <c r="E5">
-        <v>16</v>
+        <v>51</v>
       </c>
       <c r="F5">
-        <v>79</v>
+        <v>67</v>
       </c>
       <c r="G5">
-        <v>87.025000000000006</v>
+        <v>78.835300000000004</v>
       </c>
       <c r="H5">
-        <v>16</v>
+        <v>58</v>
       </c>
       <c r="I5">
-        <v>79</v>
+        <v>62</v>
       </c>
       <c r="J5">
-        <v>87.025000000000006</v>
+        <v>77.826400000000007</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
@@ -561,31 +562,31 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>15</v>
+        <v>58</v>
       </c>
       <c r="C6">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="D6">
-        <v>85.523799999999994</v>
+        <v>94.962500000000006</v>
       </c>
       <c r="E6">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="F6">
-        <v>77</v>
+        <v>99</v>
       </c>
       <c r="G6">
-        <v>86.987200000000001</v>
+        <v>99</v>
       </c>
       <c r="H6">
-        <v>13</v>
+        <v>58</v>
       </c>
       <c r="I6">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="J6">
-        <v>87.012799999999999</v>
+        <v>94.962500000000006</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
@@ -593,31 +594,31 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>15</v>
+        <v>53</v>
       </c>
       <c r="C7">
-        <v>64</v>
+        <v>87</v>
       </c>
       <c r="D7">
-        <v>79.638099999999994</v>
+        <v>95.493499999999997</v>
       </c>
       <c r="E7">
-        <v>14</v>
+        <v>54</v>
       </c>
       <c r="F7">
-        <v>71</v>
+        <v>38</v>
       </c>
       <c r="G7">
-        <v>80.857100000000003</v>
+        <v>93.478700000000003</v>
       </c>
       <c r="H7">
-        <v>16</v>
+        <v>53</v>
       </c>
       <c r="I7">
-        <v>44</v>
+        <v>87</v>
       </c>
       <c r="J7">
-        <v>75.866699999999994</v>
+        <v>95.493499999999997</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
@@ -625,31 +626,31 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>14</v>
+        <v>48</v>
       </c>
       <c r="C8">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D8">
-        <v>86.813199999999995</v>
+        <v>77.377700000000004</v>
       </c>
       <c r="E8">
-        <v>5</v>
+        <v>48</v>
       </c>
       <c r="F8">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="G8">
-        <v>84.8</v>
+        <v>77.370599999999996</v>
       </c>
       <c r="H8">
-        <v>15</v>
+        <v>48</v>
       </c>
       <c r="I8">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="J8">
-        <v>85.6</v>
+        <v>77.377700000000004</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
@@ -657,31 +658,31 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <v>13</v>
+        <v>48</v>
       </c>
       <c r="C9">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D9">
-        <v>89.2821</v>
+        <v>77.944100000000006</v>
       </c>
       <c r="E9">
-        <v>12</v>
+        <v>47</v>
       </c>
       <c r="F9">
-        <v>86</v>
+        <v>65</v>
       </c>
       <c r="G9">
-        <v>93.090900000000005</v>
+        <v>78.265500000000003</v>
       </c>
       <c r="H9">
-        <v>12</v>
+        <v>48</v>
       </c>
       <c r="I9">
-        <v>86</v>
+        <v>65</v>
       </c>
       <c r="J9">
-        <v>93.090900000000005</v>
+        <v>77.944100000000006</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
@@ -689,31 +690,31 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>13</v>
+        <v>45</v>
       </c>
       <c r="C10">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="D10">
-        <v>79.602599999999995</v>
+        <v>74.324200000000005</v>
       </c>
       <c r="E10">
-        <v>13</v>
+        <v>45</v>
       </c>
       <c r="F10">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="G10">
-        <v>79.602599999999995</v>
+        <v>74.402000000000001</v>
       </c>
       <c r="H10">
-        <v>13</v>
+        <v>45</v>
       </c>
       <c r="I10">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="J10">
-        <v>79.602599999999995</v>
+        <v>74.324200000000005</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
@@ -721,31 +722,31 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>13</v>
+        <v>45</v>
       </c>
       <c r="C11">
-        <v>56</v>
+        <v>67</v>
       </c>
       <c r="D11">
-        <v>79.935900000000004</v>
+        <v>88.623199999999997</v>
       </c>
       <c r="E11">
-        <v>1</v>
+        <v>54</v>
       </c>
       <c r="F11">
-        <v>0</v>
+        <v>68</v>
       </c>
       <c r="G11">
-        <v>0</v>
+        <v>88.3536</v>
       </c>
       <c r="H11">
-        <v>11</v>
+        <v>45</v>
       </c>
       <c r="I11">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="J11">
-        <v>84.018199999999993</v>
+        <v>88.623199999999997</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
@@ -753,31 +754,31 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>12</v>
+        <v>45</v>
       </c>
       <c r="C12">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="D12">
-        <v>88.212100000000007</v>
+        <v>92.509100000000004</v>
       </c>
       <c r="E12">
-        <v>12</v>
+        <v>45</v>
       </c>
       <c r="F12">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="G12">
-        <v>88.212100000000007</v>
+        <v>92.509100000000004</v>
       </c>
       <c r="H12">
-        <v>12</v>
+        <v>45</v>
       </c>
       <c r="I12">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="J12">
-        <v>88.212100000000007</v>
+        <v>92.509100000000004</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
@@ -785,31 +786,31 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>12</v>
+        <v>41</v>
       </c>
       <c r="C13">
         <v>64</v>
       </c>
       <c r="D13">
-        <v>77.651499999999999</v>
+        <v>76.596299999999999</v>
       </c>
       <c r="E13">
-        <v>6</v>
+        <v>109</v>
       </c>
       <c r="F13">
-        <v>75</v>
+        <v>58</v>
       </c>
       <c r="G13">
-        <v>81.133300000000006</v>
+        <v>77.043199999999999</v>
       </c>
       <c r="H13">
-        <v>3</v>
+        <v>55</v>
       </c>
       <c r="I13">
-        <v>73</v>
+        <v>59</v>
       </c>
       <c r="J13">
-        <v>75.333299999999994</v>
+        <v>75.931299999999993</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
@@ -817,31 +818,31 @@
         <v>12</v>
       </c>
       <c r="B14">
-        <v>10</v>
+        <v>41</v>
       </c>
       <c r="C14">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="D14">
-        <v>81.599999999999994</v>
+        <v>74.579300000000003</v>
       </c>
       <c r="E14">
-        <v>4</v>
+        <v>43</v>
       </c>
       <c r="F14">
-        <v>77</v>
+        <v>65</v>
       </c>
       <c r="G14">
-        <v>85</v>
+        <v>74.503900000000002</v>
       </c>
       <c r="H14">
-        <v>7</v>
+        <v>41</v>
       </c>
       <c r="I14">
-        <v>57</v>
+        <v>65</v>
       </c>
       <c r="J14">
-        <v>68.428600000000003</v>
+        <v>74.579300000000003</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
@@ -849,31 +850,31 @@
         <v>13</v>
       </c>
       <c r="B15">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="C15">
-        <v>79</v>
+        <v>66</v>
       </c>
       <c r="D15">
-        <v>89.777799999999999</v>
+        <v>78.339699999999993</v>
       </c>
       <c r="E15">
-        <v>10</v>
+        <v>109</v>
       </c>
       <c r="F15">
-        <v>79</v>
+        <v>58</v>
       </c>
       <c r="G15">
-        <v>89.777799999999999</v>
+        <v>77.043199999999999</v>
       </c>
       <c r="H15">
-        <v>10</v>
+        <v>55</v>
       </c>
       <c r="I15">
-        <v>79</v>
+        <v>59</v>
       </c>
       <c r="J15">
-        <v>89.777799999999999</v>
+        <v>75.931299999999993</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
@@ -881,31 +882,31 @@
         <v>14</v>
       </c>
       <c r="B16">
-        <v>10</v>
+        <v>39</v>
       </c>
       <c r="C16">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="D16">
-        <v>77.222200000000001</v>
+        <v>78.264499999999998</v>
       </c>
       <c r="E16">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F16">
-        <v>77</v>
+        <v>89</v>
       </c>
       <c r="G16">
-        <v>85.333299999999994</v>
+        <v>92</v>
       </c>
       <c r="H16">
-        <v>10</v>
+        <v>39</v>
       </c>
       <c r="I16">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="J16">
-        <v>77.222200000000001</v>
+        <v>78.264499999999998</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
@@ -913,31 +914,31 @@
         <v>15</v>
       </c>
       <c r="B17">
-        <v>9</v>
+        <v>39</v>
       </c>
       <c r="C17">
-        <v>98</v>
+        <v>68</v>
       </c>
       <c r="D17">
-        <v>98.833299999999994</v>
+        <v>76.983800000000002</v>
       </c>
       <c r="E17">
-        <v>9</v>
+        <v>26</v>
       </c>
       <c r="F17">
-        <v>98</v>
+        <v>69</v>
       </c>
       <c r="G17">
-        <v>98.833299999999994</v>
+        <v>78.104600000000005</v>
       </c>
       <c r="H17">
-        <v>9</v>
+        <v>39</v>
       </c>
       <c r="I17">
-        <v>98</v>
+        <v>68</v>
       </c>
       <c r="J17">
-        <v>98.833299999999994</v>
+        <v>76.983800000000002</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
@@ -945,31 +946,31 @@
         <v>16</v>
       </c>
       <c r="B18">
-        <v>9</v>
+        <v>38</v>
       </c>
       <c r="C18">
-        <v>56</v>
+        <v>69</v>
       </c>
       <c r="D18">
-        <v>70.972200000000001</v>
+        <v>92.779499999999999</v>
       </c>
       <c r="E18">
-        <v>9</v>
+        <v>53</v>
       </c>
       <c r="F18">
-        <v>56</v>
+        <v>26</v>
       </c>
       <c r="G18">
-        <v>70.972200000000001</v>
+        <v>76.9499</v>
       </c>
       <c r="H18">
-        <v>15</v>
+        <v>38</v>
       </c>
       <c r="I18">
-        <v>6</v>
+        <v>69</v>
       </c>
       <c r="J18">
-        <v>52.352400000000003</v>
+        <v>92.779499999999999</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
@@ -977,31 +978,31 @@
         <v>17</v>
       </c>
       <c r="B19">
-        <v>9</v>
+        <v>38</v>
       </c>
       <c r="C19">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="D19">
-        <v>76.805599999999998</v>
+        <v>92.186300000000003</v>
       </c>
       <c r="E19">
-        <v>9</v>
+        <v>38</v>
       </c>
       <c r="F19">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="G19">
-        <v>76.805599999999998</v>
+        <v>92.186300000000003</v>
       </c>
       <c r="H19">
-        <v>9</v>
+        <v>38</v>
       </c>
       <c r="I19">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="J19">
-        <v>76.805599999999998</v>
+        <v>92.186300000000003</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
@@ -1009,31 +1010,31 @@
         <v>18</v>
       </c>
       <c r="B20">
-        <v>8</v>
+        <v>38</v>
       </c>
       <c r="C20">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D20">
-        <v>90.142899999999997</v>
+        <v>95.864900000000006</v>
       </c>
       <c r="E20">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="F20">
-        <v>83</v>
+        <v>67</v>
       </c>
       <c r="G20">
-        <v>90.142899999999997</v>
+        <v>91.947699999999998</v>
       </c>
       <c r="H20">
-        <v>8</v>
+        <v>54</v>
       </c>
       <c r="I20">
-        <v>83</v>
+        <v>65</v>
       </c>
       <c r="J20">
-        <v>90.142899999999997</v>
+        <v>95.222899999999996</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
@@ -1041,31 +1042,31 @@
         <v>19</v>
       </c>
       <c r="B21">
-        <v>8</v>
+        <v>37</v>
       </c>
       <c r="C21">
-        <v>69</v>
+        <v>78</v>
       </c>
       <c r="D21">
-        <v>82.357100000000003</v>
+        <v>88.573599999999999</v>
       </c>
       <c r="E21">
-        <v>8</v>
+        <v>37</v>
       </c>
       <c r="F21">
-        <v>69</v>
+        <v>78</v>
       </c>
       <c r="G21">
-        <v>82.357100000000003</v>
+        <v>88.573599999999999</v>
       </c>
       <c r="H21">
-        <v>6</v>
+        <v>37</v>
       </c>
       <c r="I21">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="J21">
-        <v>88.2667</v>
+        <v>88.573599999999999</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
@@ -1073,31 +1074,31 @@
         <v>20</v>
       </c>
       <c r="B22">
-        <v>8</v>
+        <v>36</v>
       </c>
       <c r="C22">
-        <v>74</v>
+        <v>95</v>
       </c>
       <c r="D22">
-        <v>82.607100000000003</v>
+        <v>97.572999999999993</v>
       </c>
       <c r="E22">
-        <v>8</v>
+        <v>53</v>
       </c>
       <c r="F22">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="G22">
-        <v>82.607100000000003</v>
+        <v>88.125500000000002</v>
       </c>
       <c r="H22">
-        <v>8</v>
+        <v>53</v>
       </c>
       <c r="I22">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="J22">
-        <v>82.607100000000003</v>
+        <v>88.125500000000002</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
@@ -1105,31 +1106,31 @@
         <v>21</v>
       </c>
       <c r="B23">
-        <v>8</v>
+        <v>36</v>
       </c>
       <c r="C23">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D23">
-        <v>82.392899999999997</v>
+        <v>78.966700000000003</v>
       </c>
       <c r="E23">
-        <v>5</v>
+        <v>36</v>
       </c>
       <c r="F23">
-        <v>81</v>
+        <v>63</v>
       </c>
       <c r="G23">
-        <v>88.4</v>
+        <v>78.365099999999998</v>
       </c>
       <c r="H23">
-        <v>8</v>
+        <v>36</v>
       </c>
       <c r="I23">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="J23">
-        <v>82.392899999999997</v>
+        <v>78.966700000000003</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
@@ -1137,31 +1138,31 @@
         <v>22</v>
       </c>
       <c r="B24">
-        <v>8</v>
+        <v>36</v>
       </c>
       <c r="C24">
-        <v>76</v>
+        <v>81</v>
       </c>
       <c r="D24">
-        <v>87.25</v>
+        <v>90.963499999999996</v>
       </c>
       <c r="E24">
-        <v>8</v>
+        <v>36</v>
       </c>
       <c r="F24">
-        <v>76</v>
+        <v>81</v>
       </c>
       <c r="G24">
-        <v>87.25</v>
+        <v>90.963499999999996</v>
       </c>
       <c r="H24">
-        <v>7</v>
+        <v>36</v>
       </c>
       <c r="I24">
-        <v>76</v>
+        <v>81</v>
       </c>
       <c r="J24">
-        <v>86.714299999999994</v>
+        <v>90.963499999999996</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
@@ -1169,31 +1170,31 @@
         <v>23</v>
       </c>
       <c r="B25">
-        <v>7</v>
+        <v>34</v>
       </c>
       <c r="C25">
-        <v>67</v>
+        <v>83</v>
       </c>
       <c r="D25">
-        <v>76.571399999999997</v>
+        <v>95.739800000000002</v>
       </c>
       <c r="E25">
-        <v>7</v>
+        <v>43</v>
       </c>
       <c r="F25">
-        <v>67</v>
+        <v>22</v>
       </c>
       <c r="G25">
-        <v>76.571399999999997</v>
+        <v>84.834999999999994</v>
       </c>
       <c r="H25">
-        <v>2</v>
+        <v>42</v>
       </c>
       <c r="I25">
-        <v>54</v>
+        <v>65</v>
       </c>
       <c r="J25">
-        <v>54</v>
+        <v>87.300799999999995</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
@@ -1201,31 +1202,31 @@
         <v>24</v>
       </c>
       <c r="B26">
-        <v>7</v>
+        <v>33</v>
       </c>
       <c r="C26">
-        <v>68</v>
+        <v>79</v>
       </c>
       <c r="D26">
-        <v>82.8095</v>
+        <v>92.748099999999994</v>
       </c>
       <c r="E26">
-        <v>6</v>
+        <v>34</v>
       </c>
       <c r="F26">
         <v>79</v>
       </c>
       <c r="G26">
-        <v>88.2667</v>
+        <v>92.183599999999998</v>
       </c>
       <c r="H26">
-        <v>7</v>
+        <v>34</v>
       </c>
       <c r="I26">
-        <v>68</v>
+        <v>79</v>
       </c>
       <c r="J26">
-        <v>82.8095</v>
+        <v>92.183599999999998</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
@@ -1233,31 +1234,31 @@
         <v>25</v>
       </c>
       <c r="B27">
-        <v>7</v>
+        <v>32</v>
       </c>
       <c r="C27">
-        <v>89</v>
+        <v>75</v>
       </c>
       <c r="D27">
-        <v>92.381</v>
+        <v>87.046400000000006</v>
       </c>
       <c r="E27">
-        <v>7</v>
+        <v>32</v>
       </c>
       <c r="F27">
-        <v>89</v>
+        <v>75</v>
       </c>
       <c r="G27">
-        <v>92.381</v>
+        <v>87.046400000000006</v>
       </c>
       <c r="H27">
-        <v>7</v>
+        <v>32</v>
       </c>
       <c r="I27">
-        <v>89</v>
+        <v>75</v>
       </c>
       <c r="J27">
-        <v>92.381</v>
+        <v>87.046400000000006</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
@@ -1265,31 +1266,31 @@
         <v>26</v>
       </c>
       <c r="B28">
-        <v>7</v>
+        <v>32</v>
       </c>
       <c r="C28">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="D28">
-        <v>83.142899999999997</v>
+        <v>82.096800000000002</v>
       </c>
       <c r="E28">
-        <v>3</v>
+        <v>17</v>
       </c>
       <c r="F28">
-        <v>85</v>
+        <v>72</v>
       </c>
       <c r="G28">
-        <v>89.666700000000006</v>
+        <v>80.860299999999995</v>
       </c>
       <c r="H28">
-        <v>8</v>
+        <v>32</v>
       </c>
       <c r="I28">
-        <v>44</v>
+        <v>72</v>
       </c>
       <c r="J28">
-        <v>74.785700000000006</v>
+        <v>82.096800000000002</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
@@ -1297,31 +1298,31 @@
         <v>27</v>
       </c>
       <c r="B29">
-        <v>7</v>
+        <v>32</v>
       </c>
       <c r="C29">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="D29">
-        <v>74.666700000000006</v>
+        <v>80.637100000000004</v>
       </c>
       <c r="E29">
-        <v>4</v>
+        <v>32</v>
       </c>
       <c r="F29">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="G29">
-        <v>77.5</v>
+        <v>80.637100000000004</v>
       </c>
       <c r="H29">
-        <v>17</v>
+        <v>32</v>
       </c>
       <c r="I29">
-        <v>18</v>
+        <v>65</v>
       </c>
       <c r="J29">
-        <v>57.198500000000003</v>
+        <v>80.637100000000004</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
@@ -1329,31 +1330,31 @@
         <v>28</v>
       </c>
       <c r="B30">
-        <v>7</v>
+        <v>32</v>
       </c>
       <c r="C30">
-        <v>70</v>
+        <v>58</v>
       </c>
       <c r="D30">
-        <v>84.761899999999997</v>
+        <v>84.852800000000002</v>
       </c>
       <c r="E30">
-        <v>6</v>
+        <v>37</v>
       </c>
       <c r="F30">
-        <v>81</v>
+        <v>55</v>
       </c>
       <c r="G30">
-        <v>89.133300000000006</v>
+        <v>82.2988</v>
       </c>
       <c r="H30">
-        <v>6</v>
+        <v>32</v>
       </c>
       <c r="I30">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="J30">
-        <v>71.333299999999994</v>
+        <v>84.852800000000002</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
@@ -1361,31 +1362,31 @@
         <v>29</v>
       </c>
       <c r="B31">
-        <v>7</v>
+        <v>31</v>
       </c>
       <c r="C31">
-        <v>77</v>
+        <v>64</v>
       </c>
       <c r="D31">
-        <v>85.952399999999997</v>
+        <v>82.597800000000007</v>
       </c>
       <c r="E31">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="F31">
-        <v>77</v>
+        <v>65</v>
       </c>
       <c r="G31">
-        <v>85.952399999999997</v>
+        <v>79.264700000000005</v>
       </c>
       <c r="H31">
-        <v>7</v>
+        <v>36</v>
       </c>
       <c r="I31">
-        <v>77</v>
+        <v>63</v>
       </c>
       <c r="J31">
-        <v>85.952399999999997</v>
+        <v>83.569800000000001</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
@@ -1393,31 +1394,31 @@
         <v>30</v>
       </c>
       <c r="B32">
-        <v>7</v>
+        <v>31</v>
       </c>
       <c r="C32">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="D32">
-        <v>81.761899999999997</v>
+        <v>79.698899999999995</v>
       </c>
       <c r="E32">
-        <v>5</v>
+        <v>31</v>
       </c>
       <c r="F32">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="G32">
-        <v>84.8</v>
+        <v>79.683899999999994</v>
       </c>
       <c r="H32">
-        <v>5</v>
+        <v>31</v>
       </c>
       <c r="I32">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="J32">
-        <v>82.4</v>
+        <v>79.698899999999995</v>
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.25">
@@ -1425,31 +1426,31 @@
         <v>31</v>
       </c>
       <c r="B33">
-        <v>7</v>
+        <v>31</v>
       </c>
       <c r="C33">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D33">
-        <v>77.666700000000006</v>
+        <v>80.051599999999993</v>
       </c>
       <c r="E33">
-        <v>7</v>
+        <v>44</v>
       </c>
       <c r="F33">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="G33">
-        <v>77.666700000000006</v>
+        <v>75.993700000000004</v>
       </c>
       <c r="H33">
-        <v>6</v>
+        <v>32</v>
       </c>
       <c r="I33">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="J33">
-        <v>81</v>
+        <v>80.288300000000007</v>
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
@@ -1457,31 +1458,31 @@
         <v>32</v>
       </c>
       <c r="B34">
-        <v>7</v>
+        <v>30</v>
       </c>
       <c r="C34">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="D34">
-        <v>85.333299999999994</v>
+        <v>87.804599999999994</v>
       </c>
       <c r="E34">
-        <v>7</v>
+        <v>30</v>
       </c>
       <c r="F34">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="G34">
-        <v>85.333299999999994</v>
+        <v>87.804599999999994</v>
       </c>
       <c r="H34">
-        <v>7</v>
+        <v>30</v>
       </c>
       <c r="I34">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="J34">
-        <v>85.333299999999994</v>
+        <v>87.804599999999994</v>
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
@@ -1489,31 +1490,31 @@
         <v>33</v>
       </c>
       <c r="B35">
-        <v>7</v>
+        <v>29</v>
       </c>
       <c r="C35">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="D35">
-        <v>84.428600000000003</v>
+        <v>83.403899999999993</v>
       </c>
       <c r="E35">
-        <v>7</v>
+        <v>33</v>
       </c>
       <c r="F35">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="G35">
-        <v>84.428600000000003</v>
+        <v>80.818200000000004</v>
       </c>
       <c r="H35">
-        <v>7</v>
+        <v>29</v>
       </c>
       <c r="I35">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="J35">
-        <v>84.428600000000003</v>
+        <v>83.403899999999993</v>
       </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.25">
@@ -1521,31 +1522,31 @@
         <v>34</v>
       </c>
       <c r="B36">
-        <v>7</v>
+        <v>29</v>
       </c>
       <c r="C36">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="D36">
-        <v>83.428600000000003</v>
+        <v>77.810299999999998</v>
       </c>
       <c r="E36">
-        <v>5</v>
+        <v>31</v>
       </c>
       <c r="F36">
-        <v>80</v>
+        <v>10</v>
       </c>
       <c r="G36">
-        <v>88.2</v>
+        <v>73.320400000000006</v>
       </c>
       <c r="H36">
-        <v>7</v>
+        <v>29</v>
       </c>
       <c r="I36">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="J36">
-        <v>83.428600000000003</v>
+        <v>77.810299999999998</v>
       </c>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.25">
@@ -1553,31 +1554,31 @@
         <v>35</v>
       </c>
       <c r="B37">
-        <v>6</v>
+        <v>29</v>
       </c>
       <c r="C37">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="D37">
-        <v>86.666700000000006</v>
+        <v>87.802999999999997</v>
       </c>
       <c r="E37">
-        <v>6</v>
+        <v>31</v>
       </c>
       <c r="F37">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="G37">
-        <v>86.666700000000006</v>
+        <v>86.032300000000006</v>
       </c>
       <c r="H37">
-        <v>6</v>
+        <v>31</v>
       </c>
       <c r="I37">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="J37">
-        <v>86.666700000000006</v>
+        <v>86.032300000000006</v>
       </c>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.25">
@@ -1585,31 +1586,31 @@
         <v>36</v>
       </c>
       <c r="B38">
-        <v>6</v>
+        <v>28</v>
       </c>
       <c r="C38">
-        <v>58</v>
+        <v>68</v>
       </c>
       <c r="D38">
-        <v>76.933300000000003</v>
+        <v>78.600499999999997</v>
       </c>
       <c r="E38">
-        <v>4</v>
+        <v>28</v>
       </c>
       <c r="F38">
-        <v>82</v>
+        <v>68</v>
       </c>
       <c r="G38">
-        <v>88</v>
+        <v>78.600499999999997</v>
       </c>
       <c r="H38">
-        <v>9</v>
+        <v>28</v>
       </c>
       <c r="I38">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="J38">
-        <v>75.027799999999999</v>
+        <v>78.600499999999997</v>
       </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.25">
@@ -1617,31 +1618,31 @@
         <v>37</v>
       </c>
       <c r="B39">
-        <v>6</v>
+        <v>28</v>
       </c>
       <c r="C39">
-        <v>90</v>
+        <v>73</v>
       </c>
       <c r="D39">
-        <v>93.6</v>
+        <v>83.415300000000002</v>
       </c>
       <c r="E39">
-        <v>6</v>
+        <v>21</v>
       </c>
       <c r="F39">
-        <v>90</v>
+        <v>67</v>
       </c>
       <c r="G39">
-        <v>93.6</v>
+        <v>82.852400000000003</v>
       </c>
       <c r="H39">
-        <v>6</v>
+        <v>21</v>
       </c>
       <c r="I39">
-        <v>90</v>
+        <v>67</v>
       </c>
       <c r="J39">
-        <v>93.6</v>
+        <v>82.852400000000003</v>
       </c>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.25">
@@ -1649,31 +1650,31 @@
         <v>38</v>
       </c>
       <c r="B40">
-        <v>6</v>
+        <v>28</v>
       </c>
       <c r="C40">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="D40">
-        <v>88.333299999999994</v>
+        <v>90.454999999999998</v>
       </c>
       <c r="E40">
-        <v>6</v>
+        <v>31</v>
       </c>
       <c r="F40">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="G40">
-        <v>88.333299999999994</v>
+        <v>88.264499999999998</v>
       </c>
       <c r="H40">
-        <v>6</v>
+        <v>31</v>
       </c>
       <c r="I40">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="J40">
-        <v>88.333299999999994</v>
+        <v>88.264499999999998</v>
       </c>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.25">
@@ -1681,31 +1682,31 @@
         <v>39</v>
       </c>
       <c r="B41">
-        <v>6</v>
+        <v>28</v>
       </c>
       <c r="C41">
+        <v>72</v>
+      </c>
+      <c r="D41">
+        <v>83.465599999999995</v>
+      </c>
+      <c r="E41">
+        <v>33</v>
+      </c>
+      <c r="F41">
         <v>61</v>
       </c>
-      <c r="D41">
-        <v>71.066699999999997</v>
-      </c>
-      <c r="E41">
-        <v>1</v>
-      </c>
-      <c r="F41">
-        <v>0</v>
-      </c>
       <c r="G41">
-        <v>0</v>
+        <v>80.344700000000003</v>
       </c>
       <c r="H41">
-        <v>5</v>
+        <v>32</v>
       </c>
       <c r="I41">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="J41">
-        <v>72.099999999999994</v>
+        <v>81.231899999999996</v>
       </c>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.25">
@@ -1713,31 +1714,31 @@
         <v>40</v>
       </c>
       <c r="B42">
-        <v>6</v>
+        <v>28</v>
       </c>
       <c r="C42">
-        <v>77</v>
+        <v>66</v>
       </c>
       <c r="D42">
-        <v>84.2667</v>
+        <v>77.272499999999994</v>
       </c>
       <c r="E42">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="F42">
-        <v>79</v>
+        <v>68</v>
       </c>
       <c r="G42">
-        <v>86.4</v>
+        <v>77.366699999999994</v>
       </c>
       <c r="H42">
-        <v>6</v>
+        <v>28</v>
       </c>
       <c r="I42">
-        <v>77</v>
+        <v>66</v>
       </c>
       <c r="J42">
-        <v>84.2667</v>
+        <v>77.272499999999994</v>
       </c>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.25">
@@ -1745,31 +1746,31 @@
         <v>41</v>
       </c>
       <c r="B43">
-        <v>6</v>
+        <v>27</v>
       </c>
       <c r="C43">
-        <v>79</v>
+        <v>66</v>
       </c>
       <c r="D43">
-        <v>84.466700000000003</v>
+        <v>83.458699999999993</v>
       </c>
       <c r="E43">
-        <v>6</v>
+        <v>28</v>
       </c>
       <c r="F43">
-        <v>79</v>
+        <v>67</v>
       </c>
       <c r="G43">
-        <v>84.466700000000003</v>
+        <v>81.550299999999993</v>
       </c>
       <c r="H43">
-        <v>7</v>
+        <v>31</v>
       </c>
       <c r="I43">
-        <v>35</v>
+        <v>62</v>
       </c>
       <c r="J43">
-        <v>71.1905</v>
+        <v>80.864500000000007</v>
       </c>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.25">
@@ -1777,31 +1778,31 @@
         <v>42</v>
       </c>
       <c r="B44">
-        <v>6</v>
+        <v>27</v>
       </c>
       <c r="C44">
         <v>77</v>
       </c>
       <c r="D44">
-        <v>87.133300000000006</v>
+        <v>90.6952</v>
       </c>
       <c r="E44">
-        <v>6</v>
+        <v>27</v>
       </c>
       <c r="F44">
         <v>77</v>
       </c>
       <c r="G44">
-        <v>87.133300000000006</v>
+        <v>90.6952</v>
       </c>
       <c r="H44">
-        <v>6</v>
+        <v>27</v>
       </c>
       <c r="I44">
         <v>77</v>
       </c>
       <c r="J44">
-        <v>87.133300000000006</v>
+        <v>90.6952</v>
       </c>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.25">
@@ -1809,31 +1810,31 @@
         <v>43</v>
       </c>
       <c r="B45">
-        <v>6</v>
+        <v>27</v>
       </c>
       <c r="C45">
-        <v>59</v>
+        <v>67</v>
       </c>
       <c r="D45">
-        <v>71.7333</v>
+        <v>82.960099999999997</v>
       </c>
       <c r="E45">
-        <v>2</v>
+        <v>26</v>
       </c>
       <c r="F45">
-        <v>92</v>
+        <v>69</v>
       </c>
       <c r="G45">
-        <v>92</v>
+        <v>84.0154</v>
       </c>
       <c r="H45">
-        <v>5</v>
+        <v>27</v>
       </c>
       <c r="I45">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="J45">
-        <v>76</v>
+        <v>82.960099999999997</v>
       </c>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.25">
@@ -1841,31 +1842,31 @@
         <v>44</v>
       </c>
       <c r="B46">
-        <v>6</v>
+        <v>27</v>
       </c>
       <c r="C46">
-        <v>86</v>
+        <v>73</v>
       </c>
       <c r="D46">
-        <v>91.8</v>
+        <v>80.546999999999997</v>
       </c>
       <c r="E46">
-        <v>6</v>
+        <v>27</v>
       </c>
       <c r="F46">
-        <v>86</v>
+        <v>73</v>
       </c>
       <c r="G46">
-        <v>91.8</v>
+        <v>80.546999999999997</v>
       </c>
       <c r="H46">
-        <v>6</v>
+        <v>27</v>
       </c>
       <c r="I46">
-        <v>86</v>
+        <v>73</v>
       </c>
       <c r="J46">
-        <v>91.8</v>
+        <v>80.546999999999997</v>
       </c>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.25">
@@ -1873,31 +1874,31 @@
         <v>45</v>
       </c>
       <c r="B47">
-        <v>6</v>
+        <v>26</v>
       </c>
       <c r="C47">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D47">
-        <v>79.866699999999994</v>
+        <v>77.5077</v>
       </c>
       <c r="E47">
-        <v>6</v>
+        <v>26</v>
       </c>
       <c r="F47">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="G47">
-        <v>79.866699999999994</v>
+        <v>77.5077</v>
       </c>
       <c r="H47">
-        <v>6</v>
+        <v>26</v>
       </c>
       <c r="I47">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="J47">
-        <v>79.933300000000003</v>
+        <v>77.5077</v>
       </c>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.25">
@@ -1905,31 +1906,31 @@
         <v>46</v>
       </c>
       <c r="B48">
-        <v>6</v>
+        <v>26</v>
       </c>
       <c r="C48">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="D48">
-        <v>75.933300000000003</v>
+        <v>87.113799999999998</v>
       </c>
       <c r="E48">
-        <v>6</v>
+        <v>27</v>
       </c>
       <c r="F48">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="G48">
-        <v>75.933300000000003</v>
+        <v>87.207999999999998</v>
       </c>
       <c r="H48">
-        <v>6</v>
+        <v>28</v>
       </c>
       <c r="I48">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="J48">
-        <v>75.933300000000003</v>
+        <v>87.328000000000003</v>
       </c>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.25">
@@ -1937,31 +1938,31 @@
         <v>47</v>
       </c>
       <c r="B49">
-        <v>6</v>
+        <v>26</v>
       </c>
       <c r="C49">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D49">
-        <v>82.466700000000003</v>
+        <v>84.273799999999994</v>
       </c>
       <c r="E49">
-        <v>5</v>
+        <v>31</v>
       </c>
       <c r="F49">
-        <v>85</v>
+        <v>67</v>
       </c>
       <c r="G49">
-        <v>88.2</v>
+        <v>81.402199999999993</v>
       </c>
       <c r="H49">
-        <v>4</v>
+        <v>31</v>
       </c>
       <c r="I49">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="J49">
-        <v>79.5</v>
+        <v>81.608599999999996</v>
       </c>
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.25">
@@ -1969,31 +1970,31 @@
         <v>48</v>
       </c>
       <c r="B50">
-        <v>6</v>
+        <v>26</v>
       </c>
       <c r="C50">
-        <v>81</v>
+        <v>65</v>
       </c>
       <c r="D50">
-        <v>87</v>
+        <v>74.624600000000001</v>
       </c>
       <c r="E50">
-        <v>6</v>
+        <v>24</v>
       </c>
       <c r="F50">
-        <v>81</v>
+        <v>65</v>
       </c>
       <c r="G50">
-        <v>87</v>
+        <v>75.579700000000003</v>
       </c>
       <c r="H50">
-        <v>6</v>
+        <v>26</v>
       </c>
       <c r="I50">
-        <v>81</v>
+        <v>65</v>
       </c>
       <c r="J50">
-        <v>87</v>
+        <v>74.624600000000001</v>
       </c>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.25">
@@ -2001,31 +2002,31 @@
         <v>49</v>
       </c>
       <c r="B51">
-        <v>6</v>
+        <v>25</v>
       </c>
       <c r="C51">
-        <v>87</v>
+        <v>69</v>
       </c>
       <c r="D51">
-        <v>90.866699999999994</v>
+        <v>80.47</v>
       </c>
       <c r="E51">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="F51">
-        <v>87</v>
+        <v>68</v>
       </c>
       <c r="G51">
-        <v>90.866699999999994</v>
+        <v>76.290899999999993</v>
       </c>
       <c r="H51">
-        <v>6</v>
+        <v>44</v>
       </c>
       <c r="I51">
-        <v>87</v>
+        <v>60</v>
       </c>
       <c r="J51">
-        <v>90.866699999999994</v>
+        <v>75.6554</v>
       </c>
     </row>
   </sheetData>

</xml_diff>